<commit_message>
edited scripts for data wrangling with ALSPAC data; excluded twins; still need to fit section on exploring structure of missing data
</commit_message>
<xml_diff>
--- a/data/generated_variables.xlsx
+++ b/data/generated_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmaj\Documents\Poor comprehenders SDAI\WP1 - Identification\ESRC_EJ_WP1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E927CB9B-D46C-4EEA-BC63-E16C2C65B867}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69687D68-A0D2-43A3-A4B0-73E9D6E5F219}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30810" yWindow="1590" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>workpack</t>
   </si>
@@ -78,6 +78,33 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>wold_vcb_raw_f8</t>
+  </si>
+  <si>
+    <t>WP1_DataExtraction.Rmd</t>
+  </si>
+  <si>
+    <t>teach_ctr_diff_f8</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>expressive vocabulary</t>
+  </si>
+  <si>
+    <t>WOLD Expressive Vocabulary</t>
+  </si>
+  <si>
+    <t>attention</t>
+  </si>
+  <si>
+    <t>TEACh Attentional Control</t>
+  </si>
+  <si>
+    <t>executive function</t>
   </si>
 </sst>
 </file>
@@ -455,9 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -540,13 +565,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q4:Q5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -606,6 +637,58 @@
         <v>18</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
edited CFA script to test auxiliary variable implementation; edited LPA scripts to remove covariances where necessary; ran preliminary LPA  models
</commit_message>
<xml_diff>
--- a/data/generated_variables.xlsx
+++ b/data/generated_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmaj\Documents\Poor comprehenders SDAI\WP1 - Identification\ESRC_EJ_WP1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69687D68-A0D2-43A3-A4B0-73E9D6E5F219}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5ECA69-3CD2-431C-9CA1-FA3FE87F2FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33750" yWindow="1380" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>workpack</t>
   </si>
@@ -77,7 +77,13 @@
     <t>for new_vars sheet, the name of the R script where new variable was created - to be updated as progress through each workpackage</t>
   </si>
   <si>
-    <t>test</t>
+    <t>language</t>
+  </si>
+  <si>
+    <t>expressive vocabulary</t>
+  </si>
+  <si>
+    <t>WOLD Expressive Vocabulary</t>
   </si>
   <si>
     <t>wold_vcb_raw_f8</t>
@@ -86,25 +92,58 @@
     <t>WP1_DataExtraction.Rmd</t>
   </si>
   <si>
+    <t>executive function</t>
+  </si>
+  <si>
+    <t>attention</t>
+  </si>
+  <si>
+    <t>TEACh Attentional Control</t>
+  </si>
+  <si>
     <t>teach_ctr_diff_f8</t>
   </si>
   <si>
-    <t>language</t>
-  </si>
-  <si>
-    <t>expressive vocabulary</t>
-  </si>
-  <si>
-    <t>WOLD Expressive Vocabulary</t>
-  </si>
-  <si>
-    <t>attention</t>
-  </si>
-  <si>
-    <t>TEACh Attentional Control</t>
-  </si>
-  <si>
-    <t>executive function</t>
+    <t>sex_fem</t>
+  </si>
+  <si>
+    <t>m_home_own</t>
+  </si>
+  <si>
+    <t>m_edu_alev</t>
+  </si>
+  <si>
+    <t>ethn_white</t>
+  </si>
+  <si>
+    <t>demographic</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>is female</t>
+  </si>
+  <si>
+    <t>maternal home ownership</t>
+  </si>
+  <si>
+    <t>home is owned/mortgaged</t>
+  </si>
+  <si>
+    <t>maternal education</t>
+  </si>
+  <si>
+    <t>has A-level or higher qualification</t>
+  </si>
+  <si>
+    <t>ethnicity</t>
+  </si>
+  <si>
+    <t>is white</t>
+  </si>
+  <si>
+    <t>Note</t>
   </si>
 </sst>
 </file>
@@ -565,21 +604,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -607,86 +647,140 @@
       <c r="I1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3">
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>